<commit_message>
upload edits of 20231008
</commit_message>
<xml_diff>
--- a/output/Table 1.xlsx
+++ b/output/Table 1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="84" uniqueCount="24">
   <si>
     <t>Measure</t>
   </si>
@@ -79,12 +79,18 @@
   </si>
   <si>
     <t>Relative change (%)</t>
+  </si>
+  <si>
+    <t>Relative change (%) Lower UL</t>
+  </si>
+  <si>
+    <t>Relative change (%) Upper UL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -121,8 +127,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -156,6 +165,12 @@
       <c r="J1" t="s">
         <v>21</v>
       </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -167,26 +182,32 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <v>26638</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2">
         <v>23670.19921875</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>29975.19921875</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>27335.900390625</v>
       </c>
-      <c r="H2" s="0">
+      <c r="H2">
         <v>23882.5</v>
       </c>
-      <c r="I2" s="0">
+      <c r="I2">
         <v>31173.30078125</v>
       </c>
-      <c r="J2" s="0">
+      <c r="J2">
         <v>2.5999999046325684</v>
+      </c>
+      <c r="K2">
+        <v>0.30000001192092896</v>
+      </c>
+      <c r="L2">
+        <v>4.9000000953674317</v>
       </c>
     </row>
     <row r="3">
@@ -199,26 +220,32 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3">
         <v>28559.69921875</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3">
         <v>26025.599609375</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>31454.900390625</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>28048.30078125</v>
       </c>
-      <c r="H3" s="0">
+      <c r="H3">
         <v>24952.099609375</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3">
         <v>31578.30078125</v>
       </c>
-      <c r="J3" s="0">
+      <c r="J3">
         <v>-1.7999999523162842</v>
+      </c>
+      <c r="K3">
+        <v>-4.5</v>
+      </c>
+      <c r="L3">
+        <v>0.80000001192092896</v>
       </c>
     </row>
     <row r="4">
@@ -231,26 +258,32 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>24766.400390625</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E4">
         <v>21444.400390625</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4">
         <v>28610.400390625</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G4">
         <v>26645.900390625</v>
       </c>
-      <c r="H4" s="0">
+      <c r="H4">
         <v>22855.80078125</v>
       </c>
-      <c r="I4" s="0">
+      <c r="I4">
         <v>30872</v>
       </c>
-      <c r="J4" s="0">
+      <c r="J4">
         <v>7.5999999046325684</v>
+      </c>
+      <c r="K4">
+        <v>5.4000000953674317</v>
+      </c>
+      <c r="L4">
+        <v>9.8000001907348633</v>
       </c>
     </row>
     <row r="5">
@@ -263,26 +296,32 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="0">
+      <c r="D5">
         <v>24247.5</v>
       </c>
-      <c r="E5" s="0">
+      <c r="E5">
         <v>21542.599609375</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5">
         <v>27249.900390625</v>
       </c>
-      <c r="G5" s="0">
+      <c r="G5">
         <v>19683.69921875</v>
       </c>
-      <c r="H5" s="0">
+      <c r="H5">
         <v>16877.099609375</v>
       </c>
-      <c r="I5" s="0">
+      <c r="I5">
         <v>22813.80078125</v>
       </c>
-      <c r="J5" s="0">
+      <c r="J5">
         <v>-18.799999237060547</v>
+      </c>
+      <c r="K5">
+        <v>-21.899999618530273</v>
+      </c>
+      <c r="L5">
+        <v>-16</v>
       </c>
     </row>
     <row r="6">
@@ -295,26 +334,32 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="0">
+      <c r="D6">
         <v>27614.69921875</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6">
         <v>25218</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>30358.400390625</v>
       </c>
-      <c r="G6" s="0">
+      <c r="G6">
         <v>20739.5</v>
       </c>
-      <c r="H6" s="0">
+      <c r="H6">
         <v>18213.69921875</v>
       </c>
-      <c r="I6" s="0">
+      <c r="I6">
         <v>23559.69921875</v>
       </c>
-      <c r="J6" s="0">
+      <c r="J6">
         <v>-24.899999618530273</v>
+      </c>
+      <c r="K6">
+        <v>-27.899999618530273</v>
+      </c>
+      <c r="L6">
+        <v>-22</v>
       </c>
     </row>
     <row r="7">
@@ -327,26 +372,32 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="0">
+      <c r="D7">
         <v>21468.900390625</v>
       </c>
-      <c r="E7" s="0">
+      <c r="E7">
         <v>18492.69921875</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7">
         <v>24880.19921875</v>
       </c>
-      <c r="G7" s="0">
+      <c r="G7">
         <v>18765.30078125</v>
       </c>
-      <c r="H7" s="0">
+      <c r="H7">
         <v>15692</v>
       </c>
-      <c r="I7" s="0">
+      <c r="I7">
         <v>22287.19921875</v>
       </c>
-      <c r="J7" s="0">
+      <c r="J7">
         <v>-12.600000381469727</v>
+      </c>
+      <c r="K7">
+        <v>-15.5</v>
+      </c>
+      <c r="L7">
+        <v>-10</v>
       </c>
     </row>
     <row r="8">
@@ -359,26 +410,32 @@
       <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="0">
+      <c r="D8">
         <v>15328.5</v>
       </c>
-      <c r="E8" s="0">
+      <c r="E8">
         <v>15259</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8">
         <v>15405.099609375</v>
       </c>
-      <c r="G8" s="0">
+      <c r="G8">
         <v>13773.400390625</v>
       </c>
-      <c r="H8" s="0">
+      <c r="H8">
         <v>13562.099609375</v>
       </c>
-      <c r="I8" s="0">
+      <c r="I8">
         <v>13999.400390625</v>
       </c>
-      <c r="J8" s="0">
+      <c r="J8">
         <v>-10.100000381469727</v>
+      </c>
+      <c r="K8">
+        <v>-11.600000381469727</v>
+      </c>
+      <c r="L8">
+        <v>-8.6000003814697266</v>
       </c>
     </row>
     <row r="9">
@@ -391,26 +448,32 @@
       <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="0">
+      <c r="D9">
         <v>18597.400390625</v>
       </c>
-      <c r="E9" s="0">
+      <c r="E9">
         <v>18493.400390625</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9">
         <v>18704.19921875</v>
       </c>
-      <c r="G9" s="0">
+      <c r="G9">
         <v>15825.400390625</v>
       </c>
-      <c r="H9" s="0">
+      <c r="H9">
         <v>15570.5</v>
       </c>
-      <c r="I9" s="0">
+      <c r="I9">
         <v>16099.2998046875</v>
       </c>
-      <c r="J9" s="0">
+      <c r="J9">
         <v>-14.899999618530273</v>
+      </c>
+      <c r="K9">
+        <v>-16.399999618530273</v>
+      </c>
+      <c r="L9">
+        <v>-13.399999618530273</v>
       </c>
     </row>
     <row r="10">
@@ -423,26 +486,32 @@
       <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="0">
+      <c r="D10">
         <v>12144.900390625</v>
       </c>
-      <c r="E10" s="0">
+      <c r="E10">
         <v>12071.099609375</v>
       </c>
-      <c r="F10" s="0">
+      <c r="F10">
         <v>12222.7998046875</v>
       </c>
-      <c r="G10" s="0">
+      <c r="G10">
         <v>11785.7001953125</v>
       </c>
-      <c r="H10" s="0">
+      <c r="H10">
         <v>11616.5</v>
       </c>
-      <c r="I10" s="0">
+      <c r="I10">
         <v>11965.2001953125</v>
       </c>
-      <c r="J10" s="0">
+      <c r="J10">
         <v>-3</v>
+      </c>
+      <c r="K10">
+        <v>-4.5</v>
+      </c>
+      <c r="L10">
+        <v>-1.3999999761581421</v>
       </c>
     </row>
     <row r="11">
@@ -455,26 +524,32 @@
       <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="0">
+      <c r="D11">
         <v>13932</v>
       </c>
-      <c r="E11" s="0">
+      <c r="E11">
         <v>13867.400390625</v>
       </c>
-      <c r="F11" s="0">
+      <c r="F11">
         <v>14001.400390625</v>
       </c>
-      <c r="G11" s="0">
+      <c r="G11">
         <v>8963.599609375</v>
       </c>
-      <c r="H11" s="0">
+      <c r="H11">
         <v>8772.7998046875</v>
       </c>
-      <c r="I11" s="0">
+      <c r="I11">
         <v>9171.5</v>
       </c>
-      <c r="J11" s="0">
+      <c r="J11">
         <v>-35.700000762939453</v>
+      </c>
+      <c r="K11">
+        <v>-37.099998474121094</v>
+      </c>
+      <c r="L11">
+        <v>-34.200000762939453</v>
       </c>
     </row>
     <row r="12">
@@ -487,26 +562,32 @@
       <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="0">
+      <c r="D12">
         <v>18194.19921875</v>
       </c>
-      <c r="E12" s="0">
+      <c r="E12">
         <v>18091.69921875</v>
       </c>
-      <c r="F12" s="0">
+      <c r="F12">
         <v>18298.5</v>
       </c>
-      <c r="G12" s="0">
+      <c r="G12">
         <v>10956.5</v>
       </c>
-      <c r="H12" s="0">
+      <c r="H12">
         <v>10719.2998046875</v>
       </c>
-      <c r="I12" s="0">
+      <c r="I12">
         <v>11216.099609375</v>
       </c>
-      <c r="J12" s="0">
+      <c r="J12">
         <v>-39.799999237060547</v>
+      </c>
+      <c r="K12">
+        <v>-41.200000762939453</v>
+      </c>
+      <c r="L12">
+        <v>-38.299999237060547</v>
       </c>
     </row>
     <row r="13">
@@ -519,26 +600,32 @@
       <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="0">
+      <c r="D13">
         <v>10256.400390625</v>
       </c>
-      <c r="E13" s="0">
+      <c r="E13">
         <v>10195.5</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>10320.5</v>
       </c>
-      <c r="G13" s="0">
+      <c r="G13">
         <v>7120.7001953125</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <v>6976.10009765625</v>
       </c>
-      <c r="I13" s="0">
+      <c r="I13">
         <v>7277.39990234375</v>
       </c>
-      <c r="J13" s="0">
+      <c r="J13">
         <v>-30.600000381469727</v>
+      </c>
+      <c r="K13">
+        <v>-32.099998474121094</v>
+      </c>
+      <c r="L13">
+        <v>-29</v>
       </c>
     </row>
     <row r="14">
@@ -551,26 +638,32 @@
       <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="0">
+      <c r="D14">
         <v>11309.5</v>
       </c>
-      <c r="E14" s="0">
+      <c r="E14">
         <v>8360.099609375</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14">
         <v>14702.2998046875</v>
       </c>
-      <c r="G14" s="0">
+      <c r="G14">
         <v>13562.5</v>
       </c>
-      <c r="H14" s="0">
+      <c r="H14">
         <v>10140.5</v>
       </c>
-      <c r="I14" s="0">
+      <c r="I14">
         <v>17380.19921875</v>
       </c>
-      <c r="J14" s="0">
+      <c r="J14">
         <v>19.899999618530273</v>
+      </c>
+      <c r="K14">
+        <v>17.100000381469727</v>
+      </c>
+      <c r="L14">
+        <v>23.100000381469727</v>
       </c>
     </row>
     <row r="15">
@@ -583,26 +676,32 @@
       <c r="C15" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="0">
+      <c r="D15">
         <v>9962.2998046875</v>
       </c>
-      <c r="E15" s="0">
+      <c r="E15">
         <v>7430</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15">
         <v>12867.2001953125</v>
       </c>
-      <c r="G15" s="0">
+      <c r="G15">
         <v>12222.900390625</v>
       </c>
-      <c r="H15" s="0">
+      <c r="H15">
         <v>9140.7001953125</v>
       </c>
-      <c r="I15" s="0">
+      <c r="I15">
         <v>15637.599609375</v>
       </c>
-      <c r="J15" s="0">
+      <c r="J15">
         <v>22.700000762939453</v>
+      </c>
+      <c r="K15">
+        <v>19.899999618530273</v>
+      </c>
+      <c r="L15">
+        <v>26</v>
       </c>
     </row>
     <row r="16">
@@ -615,26 +714,32 @@
       <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="0">
+      <c r="D16">
         <v>12621.5</v>
       </c>
-      <c r="E16" s="0">
+      <c r="E16">
         <v>9294.5</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16">
         <v>16503.900390625</v>
       </c>
-      <c r="G16" s="0">
+      <c r="G16">
         <v>14860.2001953125</v>
       </c>
-      <c r="H16" s="0">
+      <c r="H16">
         <v>11084.7001953125</v>
       </c>
-      <c r="I16" s="0">
+      <c r="I16">
         <v>19091.5</v>
       </c>
-      <c r="J16" s="0">
+      <c r="J16">
         <v>17.700000762939453</v>
+      </c>
+      <c r="K16">
+        <v>14.399999618530273</v>
+      </c>
+      <c r="L16">
+        <v>21.100000381469727</v>
       </c>
     </row>
     <row r="17">
@@ -647,26 +752,32 @@
       <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="0">
+      <c r="D17">
         <v>10315.5</v>
       </c>
-      <c r="E17" s="0">
+      <c r="E17">
         <v>7631.39990234375</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17">
         <v>13379.2001953125</v>
       </c>
-      <c r="G17" s="0">
+      <c r="G17">
         <v>10720.099609375</v>
       </c>
-      <c r="H17" s="0">
+      <c r="H17">
         <v>7955.2001953125</v>
       </c>
-      <c r="I17" s="0">
+      <c r="I17">
         <v>13795.900390625</v>
       </c>
-      <c r="J17" s="0">
-        <v>3.9000000953674316</v>
+      <c r="J17">
+        <v>3.9000000953674317</v>
+      </c>
+      <c r="K17">
+        <v>1.8999999761581421</v>
+      </c>
+      <c r="L17">
+        <v>6.3000001907348633</v>
       </c>
     </row>
     <row r="18">
@@ -679,26 +790,32 @@
       <c r="C18" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="0">
+      <c r="D18">
         <v>9420.5</v>
       </c>
-      <c r="E18" s="0">
+      <c r="E18">
         <v>7025.2998046875</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18">
         <v>12168.400390625</v>
       </c>
-      <c r="G18" s="0">
+      <c r="G18">
         <v>9783</v>
       </c>
-      <c r="H18" s="0">
+      <c r="H18">
         <v>7259.7998046875</v>
       </c>
-      <c r="I18" s="0">
+      <c r="I18">
         <v>12543.2998046875</v>
       </c>
-      <c r="J18" s="0">
+      <c r="J18">
         <v>3.7999999523162842</v>
+      </c>
+      <c r="K18">
+        <v>1.5</v>
+      </c>
+      <c r="L18">
+        <v>6.5999999046325684</v>
       </c>
     </row>
     <row r="19">
@@ -711,26 +828,32 @@
       <c r="C19" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="0">
+      <c r="D19">
         <v>11212.599609375</v>
       </c>
-      <c r="E19" s="0">
+      <c r="E19">
         <v>8225.7998046875</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19">
         <v>14644.2001953125</v>
       </c>
-      <c r="G19" s="0">
+      <c r="G19">
         <v>11644.5</v>
       </c>
-      <c r="H19" s="0">
+      <c r="H19">
         <v>8632.599609375</v>
       </c>
-      <c r="I19" s="0">
+      <c r="I19">
         <v>15179.5</v>
       </c>
-      <c r="J19" s="0">
-        <v>3.9000000953674316</v>
+      <c r="J19">
+        <v>3.9000000953674317</v>
+      </c>
+      <c r="K19">
+        <v>1.5</v>
+      </c>
+      <c r="L19">
+        <v>6.4000000953674317</v>
       </c>
     </row>
     <row r="20">
@@ -743,25 +866,31 @@
       <c r="C20" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="0">
+      <c r="D20">
         <v>77.400001525878906</v>
       </c>
-      <c r="E20" s="0">
+      <c r="E20">
         <v>77.400001525878906</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20">
         <v>77.5</v>
       </c>
-      <c r="G20" s="0">
+      <c r="G20">
         <v>82.199996948242188</v>
       </c>
-      <c r="H20" s="0">
+      <c r="H20">
         <v>82</v>
       </c>
-      <c r="I20" s="0">
-        <v>82.300003051757812</v>
-      </c>
-      <c r="J20" s="0">
+      <c r="I20">
+        <v>82.300003051757813</v>
+      </c>
+      <c r="J20">
+        <v>6.1999998092651367</v>
+      </c>
+      <c r="K20">
+        <v>5.9000000953674317</v>
+      </c>
+      <c r="L20">
         <v>6.1999998092651367</v>
       </c>
     </row>
@@ -775,26 +904,32 @@
       <c r="C21" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="0">
+      <c r="D21">
         <v>74.199996948242188</v>
       </c>
-      <c r="E21" s="0">
+      <c r="E21">
         <v>74.099998474121094</v>
       </c>
-      <c r="F21" s="0">
-        <v>74.300003051757812</v>
-      </c>
-      <c r="G21" s="0">
+      <c r="F21">
+        <v>74.300003051757813</v>
+      </c>
+      <c r="G21">
         <v>80</v>
       </c>
-      <c r="H21" s="0">
+      <c r="H21">
         <v>79.900001525878906</v>
       </c>
-      <c r="I21" s="0">
+      <c r="I21">
         <v>80.199996948242188</v>
       </c>
-      <c r="J21" s="0">
+      <c r="J21">
         <v>7.8000001907348633</v>
+      </c>
+      <c r="K21">
+        <v>7.8000001907348633</v>
+      </c>
+      <c r="L21">
+        <v>7.9000000953674317</v>
       </c>
     </row>
     <row r="22">
@@ -807,25 +942,31 @@
       <c r="C22" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="0">
+      <c r="D22">
         <v>80.599998474121094</v>
       </c>
-      <c r="E22" s="0">
+      <c r="E22">
         <v>80.599998474121094</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22">
         <v>80.699996948242188</v>
       </c>
-      <c r="G22" s="0">
-        <v>84.300003051757812</v>
-      </c>
-      <c r="H22" s="0">
+      <c r="G22">
+        <v>84.300003051757813</v>
+      </c>
+      <c r="H22">
         <v>84.099998474121094</v>
       </c>
-      <c r="I22" s="0">
+      <c r="I22">
         <v>84.400001525878906</v>
       </c>
-      <c r="J22" s="0">
+      <c r="J22">
+        <v>4.5999999046325684</v>
+      </c>
+      <c r="K22">
+        <v>4.3000001907348633</v>
+      </c>
+      <c r="L22">
         <v>4.5999999046325684</v>
       </c>
     </row>
@@ -839,26 +980,32 @@
       <c r="C23" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="0">
+      <c r="D23">
         <v>254.69999694824219</v>
       </c>
-      <c r="E23" s="0">
+      <c r="E23">
         <v>224.80000305175781</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23">
         <v>285.89999389648438</v>
       </c>
-      <c r="G23" s="0">
+      <c r="G23">
         <v>127.80000305175781</v>
       </c>
-      <c r="H23" s="0">
+      <c r="H23">
         <v>116.09999847412109</v>
       </c>
-      <c r="I23" s="0">
+      <c r="I23">
         <v>140.80000305175781</v>
       </c>
-      <c r="J23" s="0">
+      <c r="J23">
         <v>-49.799999237060547</v>
+      </c>
+      <c r="K23">
+        <v>-56.799999237060547</v>
+      </c>
+      <c r="L23">
+        <v>-41.200000762939453</v>
       </c>
     </row>
     <row r="24">
@@ -871,26 +1018,32 @@
       <c r="C24" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="0">
-        <v>286.60000610351562</v>
-      </c>
-      <c r="E24" s="0">
+      <c r="D24">
+        <v>286.60000610351563</v>
+      </c>
+      <c r="E24">
         <v>252.89999389648438</v>
       </c>
-      <c r="F24" s="0">
+      <c r="F24">
         <v>320.70001220703125</v>
       </c>
-      <c r="G24" s="0">
-        <v>138.60000610351562</v>
-      </c>
-      <c r="H24" s="0">
+      <c r="G24">
+        <v>138.60000610351563</v>
+      </c>
+      <c r="H24">
         <v>123.90000152587891</v>
       </c>
-      <c r="I24" s="0">
+      <c r="I24">
         <v>155.19999694824219</v>
       </c>
-      <c r="J24" s="0">
+      <c r="J24">
         <v>-51.599998474121094</v>
+      </c>
+      <c r="K24">
+        <v>-58.599998474121094</v>
+      </c>
+      <c r="L24">
+        <v>-43.099998474121094</v>
       </c>
     </row>
     <row r="25">
@@ -903,26 +1056,32 @@
       <c r="C25" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="0">
-        <v>221.10000610351562</v>
-      </c>
-      <c r="E25" s="0">
-        <v>193.10000610351562</v>
-      </c>
-      <c r="F25" s="0">
+      <c r="D25">
+        <v>221.10000610351563</v>
+      </c>
+      <c r="E25">
+        <v>193.10000610351563</v>
+      </c>
+      <c r="F25">
         <v>250.80000305175781</v>
       </c>
-      <c r="G25" s="0">
+      <c r="G25">
         <v>116.30000305175781</v>
       </c>
-      <c r="H25" s="0">
+      <c r="H25">
         <v>107.80000305175781</v>
       </c>
-      <c r="I25" s="0">
+      <c r="I25">
         <v>125.69999694824219</v>
       </c>
-      <c r="J25" s="0">
+      <c r="J25">
         <v>-47.400001525878906</v>
+      </c>
+      <c r="K25">
+        <v>-54.400001525878906</v>
+      </c>
+      <c r="L25">
+        <v>-38.599998474121094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>